<commit_message>
toggle to change to different attack
</commit_message>
<xml_diff>
--- a/Weapons.xlsx
+++ b/Weapons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FC4D66-E3E3-49D7-9504-82EBF78F956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5639E829-6AE7-4677-880D-F412AA7C4C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A0B5502-1D11-43AE-9C32-679A777A6EAB}"/>
   </bookViews>

</xml_diff>

<commit_message>
status uses apply effects
</commit_message>
<xml_diff>
--- a/Weapons.xlsx
+++ b/Weapons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Pictures\Onmyoji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08575383-71F9-431F-8587-3726F0666920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F048411E-EBA4-4342-B6CC-35EC82A8E133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A0B5502-1D11-43AE-9C32-679A777A6EAB}"/>
   </bookViews>
@@ -304,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,12 +319,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">

</xml_diff>